<commit_message>
Zip generated and documentation updates
</commit_message>
<xml_diff>
--- a/doc/personalDoc/working-hours-janeczek-mair.xlsx
+++ b/doc/personalDoc/working-hours-janeczek-mair.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Janeczek" sheetId="8" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <definedName name="SumEstJaneczek">Janeczek!$E$15</definedName>
     <definedName name="SumEstMair">Mair!$E$15</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>PHASE</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Designüberlegung - UML</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Schreiben der Server</t>
+  </si>
+  <si>
+    <t>Anfänge RMI</t>
+  </si>
+  <si>
+    <t>Vorbereiten des Codes</t>
+  </si>
+  <si>
+    <t>Least Connection</t>
   </si>
 </sst>
 </file>
@@ -434,7 +449,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -469,7 +484,6 @@
     <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -542,6 +556,15 @@
     <xf numFmtId="46" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -556,15 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -940,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -966,16 +980,16 @@
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="1"/>
@@ -987,141 +1001,161 @@
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="15.6" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>42012</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F5" s="10">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="26"/>
+      <c r="B6" s="17">
+        <v>42018</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="15.6" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="26"/>
+      <c r="B7" s="17">
+        <v>42019</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="15.6" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="25"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="26"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="25"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="15.6" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="25"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="26"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="26"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="26"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="15.6" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="26"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="27">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="26">
         <f>SUM(E5:E14)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F15" s="26">
         <f>SUM(F5:F14)</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="G15" s="28"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1"/>
@@ -1169,13 +1203,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.140625"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="6" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" style="6"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
@@ -1194,16 +1228,16 @@
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="1"/>
@@ -1216,22 +1250,22 @@
     </row>
     <row r="4" spans="1:9" ht="15.6" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="6"/>
@@ -1239,13 +1273,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1"/>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>42012</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="36" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="10">
@@ -1254,105 +1288,125 @@
       <c r="F5" s="11">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="19"/>
+      <c r="B6" s="17">
+        <v>42018</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="17">
+        <v>42019</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="19"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="19"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="19"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="20">
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="19">
         <f>SUM(E5:E14)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F15" s="20">
+        <v>0.375</v>
+      </c>
+      <c r="F15" s="19">
         <f>SUM(F5:F14)</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="G15" s="21"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1"/>
@@ -1400,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1411,65 +1465,65 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:4" ht="19.5" thickBot="1">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="9">
         <f>SumEstJaneczek</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="33">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D6" s="32">
         <f>SumActJaneczek</f>
-        <v>0.10416666666666667</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="9">
         <f>SumEstMair</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D7" s="33">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="32">
         <f>SumActMair</f>
-        <v>0.10416666666666667</v>
+        <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="34">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D8" s="36">
+        <v>0.77083333333333326</v>
+      </c>
+      <c r="D8" s="35">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>0.20833333333333334</v>
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>